<commit_message>
update sample xlsx file and readme.md
</commit_message>
<xml_diff>
--- a/inst/extdata/Generic_qHTS_Format_Example.xlsx
+++ b/inst/extdata/Generic_qHTS_Format_Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tools\git_projects\qhtsWaterfall\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273C3CBE-4F8F-4075-BD06-E9BD3BEDDE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94802455-2C09-463C-892B-F020294AC765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5892" yWindow="1440" windowWidth="31092" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="27024" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generic_qHTS_Format_Example" sheetId="1" r:id="rId1"/>
@@ -5033,24 +5033,26 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -5110,8 +5112,88 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>555854</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94EF72DB-9C26-B241-BC7F-2A15ACD6D4A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="6454" t="11184" r="3676" b="4284"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7981950" y="1155700"/>
+          <a:ext cx="5616804" cy="2971800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF">
+            <a:shade val="85000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="88900" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="55000" dist="18000" dir="5400000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="40000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="twoPt" dir="t">
+            <a:rot lat="0" lon="0" rev="7200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="25400" h="19050"/>
+          <a:contourClr>
+            <a:srgbClr val="FFFFFF"/>
+          </a:contourClr>
+        </a:sp3d>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5413,86 +5495,91 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1384"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" customWidth="1"/>
-    <col min="10" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="17" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:20" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="5">
+      <c r="J1" s="4">
         <v>-9.0117617909999996</v>
       </c>
-      <c r="K1" s="5">
+      <c r="K1" s="4">
         <v>-8.5346405440000002</v>
       </c>
-      <c r="L1" s="5">
+      <c r="L1" s="4">
         <v>-8.0575192869999999</v>
       </c>
-      <c r="M1" s="5">
+      <c r="M1" s="4">
         <v>-7.5803980309999996</v>
       </c>
-      <c r="N1" s="5">
+      <c r="N1" s="4">
         <v>-7.1032767769999996</v>
       </c>
-      <c r="O1" s="5">
+      <c r="O1" s="4">
         <v>-6.6261555220000004</v>
       </c>
-      <c r="P1" s="5">
+      <c r="P1" s="4">
         <v>-6.1490342670000002</v>
       </c>
-      <c r="Q1" s="5">
+      <c r="Q1" s="4">
         <v>-5.6719130120000001</v>
       </c>
-      <c r="R1" s="5">
+      <c r="R1" s="4">
         <v>-5.194791758</v>
       </c>
-      <c r="S1" s="5">
+      <c r="S1" s="4">
         <v>-4.7176705029999999</v>
       </c>
-      <c r="T1" s="5">
+      <c r="T1" s="4">
         <v>-4.2405492479999998</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -91228,6 +91315,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update generic qhts xlsx file
</commit_message>
<xml_diff>
--- a/inst/extdata/Generic_qHTS_Format_Example.xlsx
+++ b/inst/extdata/Generic_qHTS_Format_Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tools\git_projects\qhtsWaterfall\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273C3CBE-4F8F-4075-BD06-E9BD3BEDDE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE302248-DA1C-478B-8E58-AF85867D1F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5892" yWindow="1440" windowWidth="31092" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2232" yWindow="2232" windowWidth="23172" windowHeight="13848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generic_qHTS_Format_Example" sheetId="1" r:id="rId1"/>
@@ -5033,24 +5033,26 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -5110,8 +5112,88 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>289154</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94EF72DB-9C26-B241-BC7F-2A15ACD6D4A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="6454" t="11184" r="3676" b="4284"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5397500" y="927100"/>
+          <a:ext cx="5616804" cy="2971800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF">
+            <a:shade val="85000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="88900" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="55000" dist="18000" dir="5400000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="40000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="twoPt" dir="t">
+            <a:rot lat="0" lon="0" rev="7200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="25400" h="19050"/>
+          <a:contourClr>
+            <a:srgbClr val="FFFFFF"/>
+          </a:contourClr>
+        </a:sp3d>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5413,86 +5495,91 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1384"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" customWidth="1"/>
-    <col min="10" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="17" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:20" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="5">
+      <c r="J1" s="4">
         <v>-9.0117617909999996</v>
       </c>
-      <c r="K1" s="5">
+      <c r="K1" s="4">
         <v>-8.5346405440000002</v>
       </c>
-      <c r="L1" s="5">
+      <c r="L1" s="4">
         <v>-8.0575192869999999</v>
       </c>
-      <c r="M1" s="5">
+      <c r="M1" s="4">
         <v>-7.5803980309999996</v>
       </c>
-      <c r="N1" s="5">
+      <c r="N1" s="4">
         <v>-7.1032767769999996</v>
       </c>
-      <c r="O1" s="5">
+      <c r="O1" s="4">
         <v>-6.6261555220000004</v>
       </c>
-      <c r="P1" s="5">
+      <c r="P1" s="4">
         <v>-6.1490342670000002</v>
       </c>
-      <c r="Q1" s="5">
+      <c r="Q1" s="4">
         <v>-5.6719130120000001</v>
       </c>
-      <c r="R1" s="5">
+      <c r="R1" s="4">
         <v>-5.194791758</v>
       </c>
-      <c r="S1" s="5">
+      <c r="S1" s="4">
         <v>-4.7176705029999999</v>
       </c>
-      <c r="T1" s="5">
+      <c r="T1" s="4">
         <v>-4.2405492479999998</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -91228,6 +91315,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
example xlsx with format notes
</commit_message>
<xml_diff>
--- a/inst/extdata/Generic_qHTS_Format_Example.xlsx
+++ b/inst/extdata/Generic_qHTS_Format_Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tools\git_projects\qhtsWaterfall\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273C3CBE-4F8F-4075-BD06-E9BD3BEDDE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE302248-DA1C-478B-8E58-AF85867D1F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5892" yWindow="1440" windowWidth="31092" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2232" yWindow="2232" windowWidth="23172" windowHeight="13848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generic_qHTS_Format_Example" sheetId="1" r:id="rId1"/>
@@ -5033,24 +5033,26 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -5110,8 +5112,88 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>289154</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94EF72DB-9C26-B241-BC7F-2A15ACD6D4A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="6454" t="11184" r="3676" b="4284"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5397500" y="927100"/>
+          <a:ext cx="5616804" cy="2971800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF">
+            <a:shade val="85000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="88900" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="55000" dist="18000" dir="5400000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="40000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="twoPt" dir="t">
+            <a:rot lat="0" lon="0" rev="7200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="25400" h="19050"/>
+          <a:contourClr>
+            <a:srgbClr val="FFFFFF"/>
+          </a:contourClr>
+        </a:sp3d>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5413,86 +5495,91 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1384"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="9" max="9" width="13.88671875" customWidth="1"/>
-    <col min="10" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="17" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:20" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="5">
+      <c r="J1" s="4">
         <v>-9.0117617909999996</v>
       </c>
-      <c r="K1" s="5">
+      <c r="K1" s="4">
         <v>-8.5346405440000002</v>
       </c>
-      <c r="L1" s="5">
+      <c r="L1" s="4">
         <v>-8.0575192869999999</v>
       </c>
-      <c r="M1" s="5">
+      <c r="M1" s="4">
         <v>-7.5803980309999996</v>
       </c>
-      <c r="N1" s="5">
+      <c r="N1" s="4">
         <v>-7.1032767769999996</v>
       </c>
-      <c r="O1" s="5">
+      <c r="O1" s="4">
         <v>-6.6261555220000004</v>
       </c>
-      <c r="P1" s="5">
+      <c r="P1" s="4">
         <v>-6.1490342670000002</v>
       </c>
-      <c r="Q1" s="5">
+      <c r="Q1" s="4">
         <v>-5.6719130120000001</v>
       </c>
-      <c r="R1" s="5">
+      <c r="R1" s="4">
         <v>-5.194791758</v>
       </c>
-      <c r="S1" s="5">
+      <c r="S1" s="4">
         <v>-4.7176705029999999</v>
       </c>
-      <c r="T1" s="5">
+      <c r="T1" s="4">
         <v>-4.2405492479999998</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" s="5" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -91228,6 +91315,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>